<commit_message>
set the class strings
</commit_message>
<xml_diff>
--- a/hierarchy/uploads/upload-template.xlsx
+++ b/hierarchy/uploads/upload-template.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Igor Item Class</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>New Subproduct</t>
+  </si>
+  <si>
+    <t>NM7</t>
+  </si>
+  <si>
+    <t>New Subproduct2</t>
   </si>
 </sst>
 </file>
@@ -243,9 +249,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -270,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -279,6 +287,7 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -287,6 +296,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Product_Hierarchy" xfId="1"/>
   </cellStyles>
@@ -587,11 +597,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -629,6 +639,17 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>